<commit_message>
-revise temperature values for coldest tests -new regression output
</commit_message>
<xml_diff>
--- a/data/sig_t-output.xlsx
+++ b/data/sig_t-output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="110">
   <si>
     <t>ID</t>
   </si>
@@ -80,6 +80,27 @@
   </si>
   <si>
     <t>quality</t>
+  </si>
+  <si>
+    <t>Unnamed: 23</t>
+  </si>
+  <si>
+    <t>Unnamed: 24</t>
+  </si>
+  <si>
+    <t>Unnamed: 25</t>
+  </si>
+  <si>
+    <t>Unnamed: 26</t>
+  </si>
+  <si>
+    <t>Unnamed: 27</t>
+  </si>
+  <si>
+    <t>Unnamed: 28</t>
+  </si>
+  <si>
+    <t>Unnamed: 29</t>
   </si>
   <si>
     <t>w_rock</t>
@@ -684,13 +705,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB48"/>
+  <dimension ref="A1:AI48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -772,8 +793,29 @@
       <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="AC1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:35">
       <c r="A2" s="1">
         <v>27</v>
       </c>
@@ -781,10 +823,10 @@
         <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="E2">
         <v>100.0666666666667</v>
@@ -829,34 +871,34 @@
         <v>385.3052398299999</v>
       </c>
       <c r="S2">
-        <v>1.147730303591958</v>
+        <v>1.147712435964839</v>
       </c>
       <c r="T2" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U2" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="W2" t="s">
-        <v>102</v>
-      </c>
-      <c r="X2">
+        <v>109</v>
+      </c>
+      <c r="AE2">
         <v>27.94852486308611</v>
       </c>
-      <c r="Y2">
-        <v>10.7494326396485</v>
-      </c>
-      <c r="Z2">
+      <c r="AF2">
+        <v>9.867979163197326</v>
+      </c>
+      <c r="AG2">
         <v>2.796715721299483</v>
       </c>
-      <c r="AA2">
-        <v>0.1129765370427058</v>
-      </c>
-      <c r="AB2">
-        <v>388.1584438198208</v>
+      <c r="AH2">
+        <v>0.1037124610052039</v>
+      </c>
+      <c r="AI2">
+        <v>388.153811781802</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:35">
       <c r="A3" s="1">
         <v>28</v>
       </c>
@@ -864,10 +906,10 @@
         <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E3">
         <v>102.02</v>
@@ -912,34 +954,34 @@
         <v>379.761540585</v>
       </c>
       <c r="S3">
-        <v>1.113336404823571</v>
+        <v>1.113319287516183</v>
       </c>
       <c r="T3" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U3" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="W3" t="s">
-        <v>102</v>
-      </c>
-      <c r="X3">
+        <v>109</v>
+      </c>
+      <c r="AE3">
         <v>28.03087866541393</v>
       </c>
-      <c r="Y3">
-        <v>10.78110717900536</v>
-      </c>
-      <c r="Z3">
+      <c r="AF3">
+        <v>9.897056390326918</v>
+      </c>
+      <c r="AG3">
         <v>2.859710241445529</v>
       </c>
-      <c r="AA3">
-        <v>0.1071642053593132</v>
-      </c>
-      <c r="AB3">
-        <v>382.6748329291252</v>
+      <c r="AH3">
+        <v>0.09837674051984956</v>
+      </c>
+      <c r="AI3">
+        <v>382.6704391967054</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:35">
       <c r="A4" s="1">
         <v>37</v>
       </c>
@@ -947,10 +989,10 @@
         <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E4">
         <v>97.81333333333333</v>
@@ -995,34 +1037,34 @@
         <v>443.5371275299999</v>
       </c>
       <c r="S4">
-        <v>1.370794266287512</v>
+        <v>1.370776734550207</v>
       </c>
       <c r="T4" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="W4" t="s">
-        <v>102</v>
-      </c>
-      <c r="X4">
+        <v>109</v>
+      </c>
+      <c r="AE4">
         <v>27.97596266892597</v>
       </c>
-      <c r="Y4">
-        <v>10.75998564189461</v>
-      </c>
-      <c r="Z4">
+      <c r="AF4">
+        <v>9.877666819259247</v>
+      </c>
+      <c r="AG4">
         <v>2.752927979831212</v>
       </c>
-      <c r="AA4">
-        <v>0.1102898528294197</v>
-      </c>
-      <c r="AB4">
-        <v>446.3452004362458</v>
+      <c r="AH4">
+        <v>0.1012460848974073</v>
+      </c>
+      <c r="AI4">
+        <v>446.3406785522798</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:35">
       <c r="A5" s="1">
         <v>38</v>
       </c>
@@ -1030,10 +1072,10 @@
         <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="E5">
         <v>93.92666666666666</v>
@@ -1078,37 +1120,37 @@
         <v>542.004719515</v>
       </c>
       <c r="S5">
-        <v>1.768450894574806</v>
+        <v>1.76843342805595</v>
       </c>
       <c r="T5" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U5" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V5" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="W5" t="s">
-        <v>102</v>
-      </c>
-      <c r="X5">
+        <v>109</v>
+      </c>
+      <c r="AE5">
         <v>27.85882252757645</v>
       </c>
-      <c r="Y5">
-        <v>10.71493174137555</v>
-      </c>
-      <c r="Z5">
+      <c r="AF5">
+        <v>9.83630733858276</v>
+      </c>
+      <c r="AG5">
         <v>2.616686337273497</v>
       </c>
-      <c r="AA5">
-        <v>0.1089708558097894</v>
-      </c>
-      <c r="AB5">
-        <v>544.6758912801785</v>
+      <c r="AH5">
+        <v>0.1000352456333867</v>
+      </c>
+      <c r="AI5">
+        <v>544.6714234750903</v>
       </c>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:35">
       <c r="A6" s="1">
         <v>39</v>
       </c>
@@ -1116,10 +1158,10 @@
         <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E6">
         <v>89.39999999999999</v>
@@ -1164,37 +1206,37 @@
         <v>559.032986575</v>
       </c>
       <c r="S6">
-        <v>1.830641587157543</v>
+        <v>1.830624560939667</v>
       </c>
       <c r="T6" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U6" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V6" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="W6" t="s">
-        <v>102</v>
-      </c>
-      <c r="X6">
+        <v>109</v>
+      </c>
+      <c r="AE6">
         <v>27.94603118461817</v>
       </c>
-      <c r="Y6">
-        <v>10.74847353254545</v>
-      </c>
-      <c r="Z6">
+      <c r="AF6">
+        <v>9.867098702876723</v>
+      </c>
+      <c r="AG6">
         <v>2.560042763385588</v>
       </c>
-      <c r="AA6">
-        <v>0.1058724642955727</v>
-      </c>
-      <c r="AB6">
-        <v>561.6459655705333</v>
+      <c r="AH6">
+        <v>0.09719092222333571</v>
+      </c>
+      <c r="AI6">
+        <v>561.6416247994972</v>
       </c>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:35">
       <c r="A7" s="1">
         <v>41</v>
       </c>
@@ -1202,10 +1244,10 @@
         <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="E7">
         <v>83.17</v>
@@ -1250,37 +1292,37 @@
         <v>573.2104604799999</v>
       </c>
       <c r="S7">
-        <v>1.888665337464845</v>
+        <v>1.888648140089743</v>
       </c>
       <c r="T7" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U7" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V7" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="W7" t="s">
-        <v>102</v>
-      </c>
-      <c r="X7">
+        <v>109</v>
+      </c>
+      <c r="AE7">
         <v>27.93855081673179</v>
       </c>
-      <c r="Y7">
-        <v>10.74559646797377</v>
-      </c>
-      <c r="Z7">
+      <c r="AF7">
+        <v>9.864457557599918</v>
+      </c>
+      <c r="AG7">
         <v>2.472096104767151</v>
       </c>
-      <c r="AA7">
-        <v>0.1072410527503782</v>
-      </c>
-      <c r="AB7">
-        <v>575.7361771111423</v>
+      <c r="AH7">
+        <v>0.09844728642484719</v>
+      </c>
+      <c r="AI7">
+        <v>575.7317802279795</v>
       </c>
     </row>
-    <row r="8" spans="1:28">
+    <row r="8" spans="1:35">
       <c r="A8" s="1">
         <v>42</v>
       </c>
@@ -1288,10 +1330,10 @@
         <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="E8">
         <v>100.0666666666667</v>
@@ -1336,37 +1378,37 @@
         <v>566.0143407100001</v>
       </c>
       <c r="S8">
-        <v>1.848622903941697</v>
+        <v>1.84860567087724</v>
       </c>
       <c r="T8" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U8" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V8" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="W8" t="s">
-        <v>102</v>
-      </c>
-      <c r="X8">
+        <v>109</v>
+      </c>
+      <c r="AE8">
         <v>27.94852486308611</v>
       </c>
-      <c r="Y8">
-        <v>10.7494326396485</v>
-      </c>
-      <c r="Z8">
+      <c r="AF8">
+        <v>9.867979163197326</v>
+      </c>
+      <c r="AG8">
         <v>2.796715721299483</v>
       </c>
-      <c r="AA8">
-        <v>0.1076018207228815</v>
-      </c>
-      <c r="AB8">
-        <v>568.864857341661</v>
+      <c r="AH8">
+        <v>0.09877847142360523</v>
+      </c>
+      <c r="AI8">
+        <v>568.8604456670114</v>
       </c>
     </row>
-    <row r="9" spans="1:28">
+    <row r="9" spans="1:35">
       <c r="A9" s="1">
         <v>43</v>
       </c>
@@ -1374,10 +1416,10 @@
         <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E9">
         <v>102.02</v>
@@ -1422,37 +1464,37 @@
         <v>586.48081926</v>
       </c>
       <c r="S9">
-        <v>1.921662906310688</v>
+        <v>1.921646194513485</v>
       </c>
       <c r="T9" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U9" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V9" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="W9" t="s">
-        <v>102</v>
-      </c>
-      <c r="X9">
+        <v>109</v>
+      </c>
+      <c r="AE9">
         <v>28.03087866541393</v>
       </c>
-      <c r="Y9">
-        <v>10.78110717900536</v>
-      </c>
-      <c r="Z9">
+      <c r="AF9">
+        <v>9.897056390326918</v>
+      </c>
+      <c r="AG9">
         <v>2.859710241445529</v>
       </c>
-      <c r="AA9">
-        <v>0.1038220621338216</v>
-      </c>
-      <c r="AB9">
-        <v>589.3924405325124</v>
+      <c r="AH9">
+        <v>0.09530865303884824</v>
+      </c>
+      <c r="AI9">
+        <v>589.3881838279649</v>
       </c>
     </row>
-    <row r="10" spans="1:28">
+    <row r="10" spans="1:35">
       <c r="A10" s="1">
         <v>44</v>
       </c>
@@ -1460,10 +1502,10 @@
         <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="E10">
         <v>90.51666666666667</v>
@@ -1508,37 +1550,37 @@
         <v>573.8792740099999</v>
       </c>
       <c r="S10">
-        <v>1.890837440096999</v>
+        <v>1.890820651579327</v>
       </c>
       <c r="T10" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U10" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="V10" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="W10" t="s">
-        <v>102</v>
-      </c>
-      <c r="X10">
+        <v>109</v>
+      </c>
+      <c r="AE10">
         <v>27.95101865280697</v>
       </c>
-      <c r="Y10">
-        <v>10.75039178954114</v>
-      </c>
-      <c r="Z10">
+      <c r="AF10">
+        <v>9.868859662798767</v>
+      </c>
+      <c r="AG10">
         <v>2.530033038389911</v>
       </c>
-      <c r="AA10">
-        <v>0.1039562886048628</v>
-      </c>
-      <c r="AB10">
-        <v>576.4612851926922</v>
+      <c r="AH10">
+        <v>0.09543187293926408</v>
+      </c>
+      <c r="AI10">
+        <v>576.4570229848595</v>
       </c>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:35">
       <c r="A11" s="1">
         <v>45</v>
       </c>
@@ -1546,10 +1588,10 @@
         <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="E11">
         <v>93.09666666666668</v>
@@ -1594,37 +1636,37 @@
         <v>443.2105660849999</v>
       </c>
       <c r="S11">
-        <v>1.384818438485276</v>
+        <v>1.384801308173101</v>
       </c>
       <c r="T11" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U11" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V11" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="W11" t="s">
-        <v>102</v>
-      </c>
-      <c r="X11">
+        <v>109</v>
+      </c>
+      <c r="AE11">
         <v>27.81900110411822</v>
       </c>
-      <c r="Y11">
-        <v>10.69961580927624</v>
-      </c>
-      <c r="Z11">
+      <c r="AF11">
+        <v>9.822247312915588</v>
+      </c>
+      <c r="AG11">
         <v>2.589856272789726</v>
       </c>
-      <c r="AA11">
-        <v>0.1059261965118348</v>
-      </c>
-      <c r="AB11">
-        <v>445.8533854560455</v>
+      <c r="AH11">
+        <v>0.09724024839786433</v>
+      </c>
+      <c r="AI11">
+        <v>445.8490424819886</v>
       </c>
     </row>
-    <row r="12" spans="1:28">
+    <row r="12" spans="1:35">
       <c r="A12" s="1">
         <v>46</v>
       </c>
@@ -1632,10 +1674,10 @@
         <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="E12">
         <v>93.17999999999999</v>
@@ -1680,37 +1722,37 @@
         <v>471.567475225</v>
       </c>
       <c r="S12">
-        <v>1.494210646459688</v>
+        <v>1.494193473305889</v>
       </c>
       <c r="T12" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U12" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V12" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="W12" t="s">
-        <v>102</v>
-      </c>
-      <c r="X12">
+        <v>109</v>
+      </c>
+      <c r="AE12">
         <v>27.84886450164194</v>
       </c>
-      <c r="Y12">
-        <v>10.71110173140075</v>
-      </c>
-      <c r="Z12">
+      <c r="AF12">
+        <v>9.832791389425884</v>
+      </c>
+      <c r="AG12">
         <v>2.594957194262996</v>
       </c>
-      <c r="AA12">
-        <v>0.1064683512101234</v>
-      </c>
-      <c r="AB12">
-        <v>474.215666594868</v>
+      <c r="AH12">
+        <v>0.09773794641089328</v>
+      </c>
+      <c r="AI12">
+        <v>474.2113013924684</v>
       </c>
     </row>
-    <row r="13" spans="1:28">
+    <row r="13" spans="1:35">
       <c r="A13" s="1">
         <v>47</v>
       </c>
@@ -1718,10 +1760,10 @@
         <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="E13">
         <v>94.67333333333333</v>
@@ -1766,37 +1808,37 @@
         <v>635.052176045</v>
       </c>
       <c r="S13">
-        <v>2.122200527858644</v>
+        <v>2.122183176662082</v>
       </c>
       <c r="T13" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U13" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V13" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="W13" t="s">
-        <v>102</v>
-      </c>
-      <c r="X13">
+        <v>109</v>
+      </c>
+      <c r="AE13">
         <v>27.94104416144101</v>
       </c>
-      <c r="Y13">
-        <v>10.74655544670808</v>
-      </c>
-      <c r="Z13">
+      <c r="AF13">
+        <v>9.865337900078016</v>
+      </c>
+      <c r="AG13">
         <v>2.669766769625688</v>
       </c>
-      <c r="AA13">
-        <v>0.1085402100117516</v>
-      </c>
-      <c r="AB13">
-        <v>637.7762129196316</v>
+      <c r="AH13">
+        <v>0.09963991279078796</v>
+      </c>
+      <c r="AI13">
+        <v>637.7717627710211</v>
       </c>
     </row>
-    <row r="14" spans="1:28">
+    <row r="14" spans="1:35">
       <c r="A14" s="1">
         <v>48</v>
       </c>
@@ -1804,10 +1846,10 @@
         <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="E14">
         <v>94.28000000000002</v>
@@ -1852,37 +1894,37 @@
         <v>588.7716527</v>
       </c>
       <c r="S14">
-        <v>1.945024425055441</v>
+        <v>1.945007251267919</v>
       </c>
       <c r="T14" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U14" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V14" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="W14" t="s">
-        <v>102</v>
-      </c>
-      <c r="X14">
+        <v>109</v>
+      </c>
+      <c r="AE14">
         <v>27.93107145012167</v>
       </c>
-      <c r="Y14">
-        <v>10.74271978850834</v>
-      </c>
-      <c r="Z14">
+      <c r="AF14">
+        <v>9.861816765850653</v>
+      </c>
+      <c r="AG14">
         <v>2.643675912754016</v>
       </c>
-      <c r="AA14">
-        <v>0.106997489093543</v>
-      </c>
-      <c r="AB14">
-        <v>591.4688273573008</v>
+      <c r="AH14">
+        <v>0.09822369498787252</v>
+      </c>
+      <c r="AI14">
+        <v>591.4644404602479</v>
       </c>
     </row>
-    <row r="15" spans="1:28">
+    <row r="15" spans="1:35">
       <c r="A15" s="1">
         <v>49</v>
       </c>
@@ -1890,10 +1932,10 @@
         <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="E15">
         <v>96.17666666666666</v>
@@ -1938,37 +1980,37 @@
         <v>692.43578852</v>
       </c>
       <c r="S15">
-        <v>2.344964484983252</v>
+        <v>2.344947214778976</v>
       </c>
       <c r="T15" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U15" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="V15" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="W15" t="s">
-        <v>102</v>
-      </c>
-      <c r="X15">
+        <v>109</v>
+      </c>
+      <c r="AE15">
         <v>27.95351255378077</v>
       </c>
-      <c r="Y15">
-        <v>10.75135098222337</v>
-      </c>
-      <c r="Z15">
+      <c r="AF15">
+        <v>9.869740201681056</v>
+      </c>
+      <c r="AG15">
         <v>2.688475659047455</v>
       </c>
-      <c r="AA15">
-        <v>0.1079435638615227</v>
-      </c>
-      <c r="AB15">
-        <v>695.1782359609782</v>
+      <c r="AH15">
+        <v>0.09909219162487778</v>
+      </c>
+      <c r="AI15">
+        <v>695.1738102748599</v>
       </c>
     </row>
-    <row r="16" spans="1:28">
+    <row r="16" spans="1:35">
       <c r="A16" s="1">
         <v>50</v>
       </c>
@@ -1976,10 +2018,10 @@
         <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="E16">
         <v>96.52</v>
@@ -2024,37 +2066,37 @@
         <v>612.579256905</v>
       </c>
       <c r="S16">
-        <v>2.051791417644021</v>
+        <v>2.051774106266545</v>
       </c>
       <c r="T16" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U16" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="V16" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="W16" t="s">
-        <v>102</v>
-      </c>
-      <c r="X16">
+        <v>109</v>
+      </c>
+      <c r="AE16">
         <v>27.77920816140629</v>
       </c>
-      <c r="Y16">
-        <v>10.68431083131011</v>
-      </c>
-      <c r="Z16">
+      <c r="AF16">
+        <v>9.808197343142682</v>
+      </c>
+      <c r="AG16">
         <v>2.703657732989137</v>
       </c>
-      <c r="AA16">
-        <v>0.1071636376380404</v>
-      </c>
-      <c r="AB16">
-        <v>615.3364964568082</v>
+      <c r="AH16">
+        <v>0.0983762193517211</v>
+      </c>
+      <c r="AI16">
+        <v>615.332102747665</v>
       </c>
     </row>
-    <row r="17" spans="1:28">
+    <row r="17" spans="1:35">
       <c r="A17" s="1">
         <v>51</v>
       </c>
@@ -2062,10 +2104,10 @@
         <v>53</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="E17">
         <v>98.8</v>
@@ -2110,37 +2152,37 @@
         <v>637.5734657599999</v>
       </c>
       <c r="S17">
-        <v>2.123179769024317</v>
+        <v>2.123162565755432</v>
       </c>
       <c r="T17" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U17" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V17" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="W17" t="s">
-        <v>102</v>
-      </c>
-      <c r="X17">
+        <v>109</v>
+      </c>
+      <c r="AE17">
         <v>28.00341393636858</v>
       </c>
-      <c r="Y17">
-        <v>10.77054382168022</v>
-      </c>
-      <c r="Z17">
+      <c r="AF17">
+        <v>9.887359228302445</v>
+      </c>
+      <c r="AG17">
         <v>2.767110675765701</v>
       </c>
-      <c r="AA17">
-        <v>0.1077054382168022</v>
-      </c>
-      <c r="AB17">
-        <v>640.3944291548739</v>
+      <c r="AH17">
+        <v>0.09887359228302446</v>
+      </c>
+      <c r="AI17">
+        <v>640.3900132319071</v>
       </c>
     </row>
-    <row r="18" spans="1:28">
+    <row r="18" spans="1:35">
       <c r="A18" s="1">
         <v>52</v>
       </c>
@@ -2148,10 +2190,10 @@
         <v>54</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D18" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E18">
         <v>97.81333333333333</v>
@@ -2196,37 +2238,37 @@
         <v>453.15745118</v>
       </c>
       <c r="S18">
-        <v>1.409037469195896</v>
+        <v>1.409019585410333</v>
       </c>
       <c r="T18" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U18" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V18" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="W18" t="s">
-        <v>102</v>
-      </c>
-      <c r="X18">
+        <v>109</v>
+      </c>
+      <c r="AE18">
         <v>27.97596266892597</v>
       </c>
-      <c r="Y18">
-        <v>10.75998564189461</v>
-      </c>
-      <c r="Z18">
+      <c r="AF18">
+        <v>9.877666819259247</v>
+      </c>
+      <c r="AG18">
         <v>2.752927979831212</v>
       </c>
-      <c r="AA18">
-        <v>0.1133026488091502</v>
-      </c>
-      <c r="AB18">
-        <v>455.9670304842357</v>
+      <c r="AH18">
+        <v>0.1040118316067999</v>
+      </c>
+      <c r="AI18">
+        <v>455.9623850756346</v>
       </c>
     </row>
-    <row r="19" spans="1:28">
+    <row r="19" spans="1:35">
       <c r="A19" s="1">
         <v>54</v>
       </c>
@@ -2234,10 +2276,10 @@
         <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E19">
         <v>89.39999999999999</v>
@@ -2282,37 +2324,37 @@
         <v>447.71083777</v>
       </c>
       <c r="S19">
-        <v>1.397174853492538</v>
+        <v>1.397156798888563</v>
       </c>
       <c r="T19" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U19" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V19" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="W19" t="s">
-        <v>102</v>
-      </c>
-      <c r="X19">
+        <v>109</v>
+      </c>
+      <c r="AE19">
         <v>27.94603118461817</v>
       </c>
-      <c r="Y19">
-        <v>10.74847353254545</v>
-      </c>
-      <c r="Z19">
+      <c r="AF19">
+        <v>9.867098702876723</v>
+      </c>
+      <c r="AG19">
         <v>2.560042763385588</v>
       </c>
-      <c r="AA19">
-        <v>0.1145787278569345</v>
-      </c>
-      <c r="AB19">
-        <v>450.328169897314</v>
+      <c r="AH19">
+        <v>0.1051832721726659</v>
+      </c>
+      <c r="AI19">
+        <v>450.3234721694719</v>
       </c>
     </row>
-    <row r="20" spans="1:28">
+    <row r="20" spans="1:35">
       <c r="A20" s="1">
         <v>56</v>
       </c>
@@ -2320,10 +2362,10 @@
         <v>58</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D20" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="E20">
         <v>83.17</v>
@@ -2368,37 +2410,37 @@
         <v>417.828994555</v>
       </c>
       <c r="S20">
-        <v>1.281613260889897</v>
+        <v>1.281595934598941</v>
       </c>
       <c r="T20" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U20" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V20" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="W20" t="s">
-        <v>102</v>
-      </c>
-      <c r="X20">
+        <v>109</v>
+      </c>
+      <c r="AE20">
         <v>27.93855081673179</v>
       </c>
-      <c r="Y20">
-        <v>10.74559646797377</v>
-      </c>
-      <c r="Z20">
+      <c r="AF20">
+        <v>9.864457557599918</v>
+      </c>
+      <c r="AG20">
         <v>2.472096104767151</v>
       </c>
-      <c r="AA20">
-        <v>0.1083156123971756</v>
-      </c>
-      <c r="AB20">
-        <v>420.3552484659657</v>
+      <c r="AH20">
+        <v>0.09943373218060718</v>
+      </c>
+      <c r="AI20">
+        <v>420.3508075258574</v>
       </c>
     </row>
-    <row r="21" spans="1:28">
+    <row r="21" spans="1:35">
       <c r="A21" s="1">
         <v>57</v>
       </c>
@@ -2406,10 +2448,10 @@
         <v>59</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="E21">
         <v>100.0666666666667</v>
@@ -2454,37 +2496,37 @@
         <v>414.412357695</v>
       </c>
       <c r="S21">
-        <v>1.259149162296761</v>
+        <v>1.259131445001584</v>
       </c>
       <c r="T21" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U21" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V21" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="W21" t="s">
-        <v>102</v>
-      </c>
-      <c r="X21">
+        <v>109</v>
+      </c>
+      <c r="AE21">
         <v>27.94852486308611</v>
       </c>
-      <c r="Y21">
-        <v>10.7494326396485</v>
-      </c>
-      <c r="Z21">
+      <c r="AF21">
+        <v>9.867979163197326</v>
+      </c>
+      <c r="AG21">
         <v>2.796715721299483</v>
       </c>
-      <c r="AA21">
-        <v>0.111686605125948</v>
-      </c>
-      <c r="AB21">
-        <v>417.2649167188624</v>
+      <c r="AH21">
+        <v>0.1025283035056202</v>
+      </c>
+      <c r="AI21">
+        <v>417.2603375680523</v>
       </c>
     </row>
-    <row r="22" spans="1:28">
+    <row r="22" spans="1:35">
       <c r="A22" s="1">
         <v>59</v>
       </c>
@@ -2492,10 +2534,10 @@
         <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D22" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="E22">
         <v>90.51666666666667</v>
@@ -2540,37 +2582,37 @@
         <v>431.269989045</v>
       </c>
       <c r="S22">
-        <v>1.331989484242369</v>
+        <v>1.331972021034738</v>
       </c>
       <c r="T22" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U22" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V22" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="W22" t="s">
-        <v>102</v>
-      </c>
-      <c r="X22">
+        <v>109</v>
+      </c>
+      <c r="AE22">
         <v>27.95101865280697</v>
       </c>
-      <c r="Y22">
-        <v>10.75039178954114</v>
-      </c>
-      <c r="Z22">
+      <c r="AF22">
+        <v>9.868859662798767</v>
+      </c>
+      <c r="AG22">
         <v>2.530033038389911</v>
       </c>
-      <c r="AA22">
-        <v>0.1095464923354242</v>
-      </c>
-      <c r="AB22">
-        <v>433.8547953295576</v>
+      <c r="AH22">
+        <v>0.1005636799639194</v>
+      </c>
+      <c r="AI22">
+        <v>433.8503039233719</v>
       </c>
     </row>
-    <row r="23" spans="1:28">
+    <row r="23" spans="1:35">
       <c r="A23" s="1">
         <v>61</v>
       </c>
@@ -2578,10 +2620,10 @@
         <v>63</v>
       </c>
       <c r="C23" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D23" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="E23">
         <v>93.17999999999999</v>
@@ -2626,37 +2668,37 @@
         <v>332.9171348649999</v>
       </c>
       <c r="S23">
-        <v>0.947223984674059</v>
+        <v>0.947206941851099</v>
       </c>
       <c r="T23" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U23" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V23" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="W23" t="s">
-        <v>102</v>
-      </c>
-      <c r="X23">
+        <v>109</v>
+      </c>
+      <c r="AE23">
         <v>27.84886450164194</v>
       </c>
-      <c r="Y23">
-        <v>10.71110173140075</v>
-      </c>
-      <c r="Z23">
+      <c r="AF23">
+        <v>9.832791389425884</v>
+      </c>
+      <c r="AG23">
         <v>2.594957194262996</v>
       </c>
-      <c r="AA23">
-        <v>0.1053972410369833</v>
-      </c>
-      <c r="AB23">
-        <v>335.5647906797814</v>
+      <c r="AH23">
+        <v>0.0967546672719507</v>
+      </c>
+      <c r="AI23">
+        <v>335.5604693928989</v>
       </c>
     </row>
-    <row r="24" spans="1:28">
+    <row r="24" spans="1:35">
       <c r="A24" s="1">
         <v>62</v>
       </c>
@@ -2664,10 +2706,10 @@
         <v>64</v>
       </c>
       <c r="C24" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D24" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="E24">
         <v>94.67333333333333</v>
@@ -2712,37 +2754,37 @@
         <v>434.3708517749999</v>
       </c>
       <c r="S24">
-        <v>1.338957508598737</v>
+        <v>1.338940350831915</v>
       </c>
       <c r="T24" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U24" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V24" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="W24" t="s">
-        <v>102</v>
-      </c>
-      <c r="X24">
+        <v>109</v>
+      </c>
+      <c r="AE24">
         <v>27.94104416144101</v>
       </c>
-      <c r="Y24">
-        <v>10.74655544670808</v>
-      </c>
-      <c r="Z24">
+      <c r="AF24">
+        <v>9.865337900078016</v>
+      </c>
+      <c r="AG24">
         <v>2.669766769625688</v>
       </c>
-      <c r="AA24">
-        <v>0.1069282266947454</v>
-      </c>
-      <c r="AB24">
-        <v>437.094082657973</v>
+      <c r="AH24">
+        <v>0.09816011210577624</v>
+      </c>
+      <c r="AI24">
+        <v>437.0896986006785</v>
       </c>
     </row>
-    <row r="25" spans="1:28">
+    <row r="25" spans="1:35">
       <c r="A25" s="1">
         <v>63</v>
       </c>
@@ -2750,10 +2792,10 @@
         <v>65</v>
       </c>
       <c r="C25" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="D25" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="E25">
         <v>94.28000000000002</v>
@@ -2798,37 +2840,37 @@
         <v>407.5055341</v>
       </c>
       <c r="S25">
-        <v>1.234541246214057</v>
+        <v>1.234524215437216</v>
       </c>
       <c r="T25" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U25" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V25" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="W25" t="s">
-        <v>102</v>
-      </c>
-      <c r="X25">
+        <v>109</v>
+      </c>
+      <c r="AE25">
         <v>27.93107145012167</v>
       </c>
-      <c r="Y25">
-        <v>10.74271978850834</v>
-      </c>
-      <c r="Z25">
+      <c r="AF25">
+        <v>9.861816765850653</v>
+      </c>
+      <c r="AG25">
         <v>2.643675912754016</v>
       </c>
-      <c r="AA25">
-        <v>0.1058157899168071</v>
-      </c>
-      <c r="AB25">
-        <v>410.2021179077124</v>
+      <c r="AH25">
+        <v>0.09713889514362893</v>
+      </c>
+      <c r="AI25">
+        <v>410.1977794603258</v>
       </c>
     </row>
-    <row r="26" spans="1:28">
+    <row r="26" spans="1:35">
       <c r="A26" s="1">
         <v>64</v>
       </c>
@@ -2836,10 +2878,10 @@
         <v>66</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D26" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="E26">
         <v>96.17666666666666</v>
@@ -2884,37 +2926,37 @@
         <v>489.927485355</v>
       </c>
       <c r="S26">
-        <v>1.554733590331711</v>
+        <v>1.554716384632679</v>
       </c>
       <c r="T26" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U26" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V26" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="W26" t="s">
-        <v>102</v>
-      </c>
-      <c r="X26">
+        <v>109</v>
+      </c>
+      <c r="AE26">
         <v>27.95351255378077</v>
       </c>
-      <c r="Y26">
-        <v>10.75135098222337</v>
-      </c>
-      <c r="Z26">
+      <c r="AF26">
+        <v>9.869740201681056</v>
+      </c>
+      <c r="AG26">
         <v>2.688475659047455</v>
       </c>
-      <c r="AA26">
-        <v>0.1074059963124115</v>
-      </c>
-      <c r="AB26">
-        <v>492.6696640122037</v>
+      <c r="AH26">
+        <v>0.09859870461479375</v>
+      </c>
+      <c r="AI26">
+        <v>492.6652603663549</v>
       </c>
     </row>
-    <row r="27" spans="1:28">
+    <row r="27" spans="1:35">
       <c r="A27" s="1">
         <v>66</v>
       </c>
@@ -2922,10 +2964,10 @@
         <v>68</v>
       </c>
       <c r="C27" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D27" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="E27">
         <v>98.8</v>
@@ -2970,37 +3012,37 @@
         <v>448.41691657</v>
       </c>
       <c r="S27">
-        <v>1.3862758416452</v>
+        <v>1.386258638376314</v>
       </c>
       <c r="T27" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U27" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V27" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="W27" t="s">
-        <v>102</v>
-      </c>
-      <c r="X27">
+        <v>109</v>
+      </c>
+      <c r="AE27">
         <v>28.00341393636858</v>
       </c>
-      <c r="Y27">
-        <v>10.77054382168022</v>
-      </c>
-      <c r="Z27">
+      <c r="AF27">
+        <v>9.887359228302445</v>
+      </c>
+      <c r="AG27">
         <v>2.767110675765701</v>
       </c>
-      <c r="AA27">
-        <v>0.1077054382168022</v>
-      </c>
-      <c r="AB27">
-        <v>451.2378799648741</v>
+      <c r="AH27">
+        <v>0.09887359228302446</v>
+      </c>
+      <c r="AI27">
+        <v>451.2334640419072</v>
       </c>
     </row>
-    <row r="28" spans="1:28">
+    <row r="28" spans="1:35">
       <c r="A28" s="1">
         <v>67</v>
       </c>
@@ -3008,10 +3050,10 @@
         <v>69</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D28" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E28">
         <v>97.81333333333333</v>
@@ -3056,37 +3098,37 @@
         <v>242.774408065</v>
       </c>
       <c r="S28">
-        <v>0.5847739373931257</v>
+        <v>0.5847568162583059</v>
       </c>
       <c r="T28" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U28" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V28" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="W28" t="s">
-        <v>102</v>
-      </c>
-      <c r="X28">
+        <v>109</v>
+      </c>
+      <c r="AE28">
         <v>27.97596266892597</v>
       </c>
-      <c r="Y28">
-        <v>10.75998564189461</v>
-      </c>
-      <c r="Z28">
+      <c r="AF28">
+        <v>9.877666819259247</v>
+      </c>
+      <c r="AG28">
         <v>2.752927979831212</v>
       </c>
-      <c r="AA28">
-        <v>0.1068466574240134</v>
-      </c>
-      <c r="AB28">
-        <v>245.5807593735432</v>
+      <c r="AH28">
+        <v>0.09808523151524431</v>
+      </c>
+      <c r="AI28">
+        <v>245.5763786605889</v>
       </c>
     </row>
-    <row r="29" spans="1:28">
+    <row r="29" spans="1:35">
       <c r="A29" s="1">
         <v>68</v>
       </c>
@@ -3094,10 +3136,10 @@
         <v>70</v>
       </c>
       <c r="C29" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D29" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="E29">
         <v>93.92666666666666</v>
@@ -3142,37 +3184,37 @@
         <v>269.14154792</v>
       </c>
       <c r="S29">
-        <v>0.6972060637100347</v>
+        <v>0.6971888676677268</v>
       </c>
       <c r="T29" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U29" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V29" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="W29" t="s">
-        <v>102</v>
-      </c>
-      <c r="X29">
+        <v>109</v>
+      </c>
+      <c r="AE29">
         <v>27.85882252757645</v>
       </c>
-      <c r="Y29">
-        <v>10.71493174137555</v>
-      </c>
-      <c r="Z29">
+      <c r="AF29">
+        <v>9.83630733858276</v>
+      </c>
+      <c r="AG29">
         <v>2.616686337273497</v>
       </c>
-      <c r="AA29">
-        <v>0.1067207201441005</v>
-      </c>
-      <c r="AB29">
-        <v>271.8115946173455</v>
+      <c r="AH29">
+        <v>0.09796962109228431</v>
+      </c>
+      <c r="AI29">
+        <v>271.8072190678196</v>
       </c>
     </row>
-    <row r="30" spans="1:28">
+    <row r="30" spans="1:35">
       <c r="A30" s="1">
         <v>69</v>
       </c>
@@ -3180,10 +3222,10 @@
         <v>71</v>
       </c>
       <c r="C30" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D30" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E30">
         <v>89.39999999999999</v>
@@ -3228,37 +3270,37 @@
         <v>294.10731749</v>
       </c>
       <c r="S30">
-        <v>0.7949069278500579</v>
+        <v>0.7948896682198071</v>
       </c>
       <c r="T30" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U30" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V30" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="W30" t="s">
-        <v>102</v>
-      </c>
-      <c r="X30">
+        <v>109</v>
+      </c>
+      <c r="AE30">
         <v>27.94603118461817</v>
       </c>
-      <c r="Y30">
-        <v>10.74847353254545</v>
-      </c>
-      <c r="Z30">
+      <c r="AF30">
+        <v>9.867098702876723</v>
+      </c>
+      <c r="AG30">
         <v>2.560042763385588</v>
       </c>
-      <c r="AA30">
-        <v>0.1078071895314308</v>
-      </c>
-      <c r="AB30">
-        <v>296.7212638481513</v>
+      <c r="AH30">
+        <v>0.09896699998985352</v>
+      </c>
+      <c r="AI30">
+        <v>296.7168437533805</v>
       </c>
     </row>
-    <row r="31" spans="1:28">
+    <row r="31" spans="1:35">
       <c r="A31" s="1">
         <v>70</v>
       </c>
@@ -3266,10 +3308,10 @@
         <v>72</v>
       </c>
       <c r="C31" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D31" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="E31">
         <v>90.69666666666667</v>
@@ -3314,37 +3356,37 @@
         <v>306.96579697</v>
       </c>
       <c r="S31">
-        <v>0.8442105494949582</v>
+        <v>0.8441934306465867</v>
       </c>
       <c r="T31" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U31" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V31" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="W31" t="s">
-        <v>102</v>
-      </c>
-      <c r="X31">
+        <v>109</v>
+      </c>
+      <c r="AE31">
         <v>27.94104416144101</v>
       </c>
-      <c r="Y31">
-        <v>10.74655544670808</v>
-      </c>
-      <c r="Z31">
+      <c r="AF31">
+        <v>9.865337900078016</v>
+      </c>
+      <c r="AG31">
         <v>2.534159568628828</v>
       </c>
-      <c r="AA31">
-        <v>0.1066058300313441</v>
-      </c>
-      <c r="AB31">
-        <v>309.5532594536446</v>
+      <c r="AH31">
+        <v>0.09786415196877392</v>
+      </c>
+      <c r="AI31">
+        <v>309.5488886146132</v>
       </c>
     </row>
-    <row r="32" spans="1:28">
+    <row r="32" spans="1:35">
       <c r="A32" s="1">
         <v>71</v>
       </c>
@@ -3352,10 +3394,10 @@
         <v>73</v>
       </c>
       <c r="C32" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D32" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="E32">
         <v>83.17</v>
@@ -3400,37 +3442,37 @@
         <v>292.723599175</v>
       </c>
       <c r="S32">
-        <v>0.7910342902540116</v>
+        <v>0.7910171317215936</v>
       </c>
       <c r="T32" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U32" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V32" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="W32" t="s">
-        <v>102</v>
-      </c>
-      <c r="X32">
+        <v>109</v>
+      </c>
+      <c r="AE32">
         <v>27.93855081673179</v>
       </c>
-      <c r="Y32">
-        <v>10.74559646797377</v>
-      </c>
-      <c r="Z32">
+      <c r="AF32">
+        <v>9.864457557599918</v>
+      </c>
+      <c r="AG32">
         <v>2.472096104767151</v>
       </c>
-      <c r="AA32">
-        <v>0.106918684856339</v>
-      </c>
-      <c r="AB32">
-        <v>295.2491546221953</v>
+      <c r="AH32">
+        <v>0.09815135269811917</v>
+      </c>
+      <c r="AI32">
+        <v>295.2447709561162</v>
       </c>
     </row>
-    <row r="33" spans="1:28">
+    <row r="33" spans="1:35">
       <c r="A33" s="1">
         <v>72</v>
       </c>
@@ -3438,10 +3480,10 @@
         <v>74</v>
       </c>
       <c r="C33" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D33" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="E33">
         <v>100.0666666666667</v>
@@ -3486,37 +3528,37 @@
         <v>275.64335687</v>
       </c>
       <c r="S33">
-        <v>0.7149852616772786</v>
+        <v>0.7149679899320512</v>
       </c>
       <c r="T33" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U33" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V33" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="W33" t="s">
-        <v>102</v>
-      </c>
-      <c r="X33">
+        <v>109</v>
+      </c>
+      <c r="AE33">
         <v>27.94852486308611</v>
       </c>
-      <c r="Y33">
-        <v>10.7494326396485</v>
-      </c>
-      <c r="Z33">
+      <c r="AF33">
+        <v>9.867979163197326</v>
+      </c>
+      <c r="AG33">
         <v>2.796715721299483</v>
       </c>
-      <c r="AA33">
-        <v>0.107924303702071</v>
-      </c>
-      <c r="AB33">
-        <v>278.4940347431505</v>
+      <c r="AH33">
+        <v>0.09907451079850114</v>
+      </c>
+      <c r="AI33">
+        <v>278.4896098466987</v>
       </c>
     </row>
-    <row r="34" spans="1:28">
+    <row r="34" spans="1:35">
       <c r="A34" s="1">
         <v>73</v>
       </c>
@@ -3524,10 +3566,10 @@
         <v>75</v>
       </c>
       <c r="C34" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D34" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E34">
         <v>102.02</v>
@@ -3572,37 +3614,37 @@
         <v>270.421315745</v>
       </c>
       <c r="S34">
-        <v>0.6882086281423343</v>
+        <v>0.6881914591128708</v>
       </c>
       <c r="T34" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U34" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V34" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="W34" t="s">
-        <v>102</v>
-      </c>
-      <c r="X34">
+        <v>109</v>
+      </c>
+      <c r="AE34">
         <v>28.03087866541393</v>
       </c>
-      <c r="Y34">
-        <v>10.78110717900536</v>
-      </c>
-      <c r="Z34">
+      <c r="AF34">
+        <v>9.897056390326918</v>
+      </c>
+      <c r="AG34">
         <v>2.859710241445529</v>
       </c>
-      <c r="AA34">
-        <v>0.1075954496464735</v>
-      </c>
-      <c r="AB34">
-        <v>273.3348237112688</v>
+      <c r="AH34">
+        <v>0.09877262277546266</v>
+      </c>
+      <c r="AI34">
+        <v>273.3304122978333</v>
       </c>
     </row>
-    <row r="35" spans="1:28">
+    <row r="35" spans="1:35">
       <c r="A35" s="1">
         <v>74</v>
       </c>
@@ -3610,10 +3652,10 @@
         <v>76</v>
       </c>
       <c r="C35" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D35" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="E35">
         <v>90.51666666666667</v>
@@ -3658,37 +3700,37 @@
         <v>277.55369229</v>
       </c>
       <c r="S35">
-        <v>0.7308257757773967</v>
+        <v>0.7308085305800992</v>
       </c>
       <c r="T35" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U35" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V35" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="W35" t="s">
-        <v>102</v>
-      </c>
-      <c r="X35">
+        <v>109</v>
+      </c>
+      <c r="AE35">
         <v>27.95101865280697</v>
       </c>
-      <c r="Y35">
-        <v>10.75039178954114</v>
-      </c>
-      <c r="Z35">
+      <c r="AF35">
+        <v>9.868859662798767</v>
+      </c>
+      <c r="AG35">
         <v>2.530033038389911</v>
       </c>
-      <c r="AA35">
-        <v>0.1077189257312022</v>
-      </c>
-      <c r="AB35">
-        <v>280.1375847912555</v>
+      <c r="AH35">
+        <v>0.09888597382124364</v>
+      </c>
+      <c r="AI35">
+        <v>280.1331683153006</v>
       </c>
     </row>
-    <row r="36" spans="1:28">
+    <row r="36" spans="1:35">
       <c r="A36" s="1">
         <v>75</v>
       </c>
@@ -3696,10 +3738,10 @@
         <v>77</v>
       </c>
       <c r="C36" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D36" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="E36">
         <v>93.09666666666668</v>
@@ -3744,37 +3786,37 @@
         <v>187.24032978</v>
       </c>
       <c r="S36">
-        <v>0.3775421414953159</v>
+        <v>0.377524907207725</v>
       </c>
       <c r="T36" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U36" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V36" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="W36" t="s">
-        <v>102</v>
-      </c>
-      <c r="X36">
+        <v>109</v>
+      </c>
+      <c r="AE36">
         <v>27.81900110411822</v>
       </c>
-      <c r="Y36">
-        <v>10.69961580927624</v>
-      </c>
-      <c r="Z36">
+      <c r="AF36">
+        <v>9.822247312915588</v>
+      </c>
+      <c r="AG36">
         <v>2.589856272789726</v>
       </c>
-      <c r="AA36">
-        <v>0.1067821657765769</v>
-      </c>
-      <c r="AB36">
-        <v>189.8835771356781</v>
+      <c r="AH36">
+        <v>0.09802602818289757</v>
+      </c>
+      <c r="AI36">
+        <v>189.8791990668812</v>
       </c>
     </row>
-    <row r="37" spans="1:28">
+    <row r="37" spans="1:35">
       <c r="A37" s="1">
         <v>77</v>
       </c>
@@ -3782,10 +3824,10 @@
         <v>79</v>
       </c>
       <c r="C37" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D37" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="E37">
         <v>94.67333333333333</v>
@@ -3830,37 +3872,37 @@
         <v>160.52701518</v>
       </c>
       <c r="S37">
-        <v>0.2656230978229199</v>
+        <v>0.2656060049632387</v>
       </c>
       <c r="T37" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U37" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V37" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="W37" t="s">
-        <v>102</v>
-      </c>
-      <c r="X37">
+        <v>109</v>
+      </c>
+      <c r="AE37">
         <v>27.94104416144101</v>
       </c>
-      <c r="Y37">
-        <v>10.74655544670808</v>
-      </c>
-      <c r="Z37">
+      <c r="AF37">
+        <v>9.865337900078016</v>
+      </c>
+      <c r="AG37">
         <v>2.669766769625688</v>
       </c>
-      <c r="AA37">
-        <v>0.10639089892241</v>
-      </c>
-      <c r="AB37">
-        <v>163.2499773990869</v>
+      <c r="AH37">
+        <v>0.09766684521077236</v>
+      </c>
+      <c r="AI37">
+        <v>163.2456153722311</v>
       </c>
     </row>
-    <row r="38" spans="1:28">
+    <row r="38" spans="1:35">
       <c r="A38" s="1">
         <v>78</v>
       </c>
@@ -3868,10 +3910,10 @@
         <v>80</v>
       </c>
       <c r="C38" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="D38" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="E38">
         <v>94.28000000000002</v>
@@ -3916,37 +3958,37 @@
         <v>165.64412515</v>
       </c>
       <c r="S38">
-        <v>0.2895134369394334</v>
+        <v>0.2894962243298657</v>
       </c>
       <c r="T38" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U38" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V38" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="W38" t="s">
-        <v>102</v>
-      </c>
-      <c r="X38">
+        <v>109</v>
+      </c>
+      <c r="AE38">
         <v>27.93107145012167</v>
       </c>
-      <c r="Y38">
-        <v>10.74271978850834</v>
-      </c>
-      <c r="Z38">
+      <c r="AF38">
+        <v>9.861816765850653</v>
+      </c>
+      <c r="AG38">
         <v>2.643675912754016</v>
       </c>
-      <c r="AA38">
-        <v>0.1073197706871983</v>
-      </c>
-      <c r="AB38">
-        <v>168.3414609480976</v>
+      <c r="AH38">
+        <v>0.09851954949084803</v>
+      </c>
+      <c r="AI38">
+        <v>168.3370608374994</v>
       </c>
     </row>
-    <row r="39" spans="1:28">
+    <row r="39" spans="1:35">
       <c r="A39" s="1">
         <v>79</v>
       </c>
@@ -3954,10 +3996,10 @@
         <v>81</v>
       </c>
       <c r="C39" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D39" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="E39">
         <v>96.17666666666666</v>
@@ -4002,37 +4044,37 @@
         <v>163.29052915</v>
       </c>
       <c r="S39">
-        <v>0.2762961188108836</v>
+        <v>0.276279003780786</v>
       </c>
       <c r="T39" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U39" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V39" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="W39" t="s">
-        <v>102</v>
-      </c>
-      <c r="X39">
+        <v>109</v>
+      </c>
+      <c r="AE39">
         <v>27.95351255378077</v>
       </c>
-      <c r="Y39">
-        <v>10.75135098222337</v>
-      </c>
-      <c r="Z39">
+      <c r="AF39">
+        <v>9.869740201681056</v>
+      </c>
+      <c r="AG39">
         <v>2.688475659047455</v>
       </c>
-      <c r="AA39">
-        <v>0.1066534017436559</v>
-      </c>
-      <c r="AB39">
-        <v>166.0323315099193</v>
+      <c r="AH39">
+        <v>0.09790782280067607</v>
+      </c>
+      <c r="AI39">
+        <v>166.0279587204478</v>
       </c>
     </row>
-    <row r="40" spans="1:28">
+    <row r="40" spans="1:35">
       <c r="A40" s="1">
         <v>80</v>
       </c>
@@ -4040,10 +4082,10 @@
         <v>82</v>
       </c>
       <c r="C40" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D40" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="E40">
         <v>96.52</v>
@@ -4088,37 +4130,37 @@
         <v>136.14572195</v>
       </c>
       <c r="S40">
-        <v>0.1742789342752269</v>
+        <v>0.1742616358305753</v>
       </c>
       <c r="T40" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U40" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V40" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="W40" t="s">
-        <v>102</v>
-      </c>
-      <c r="X40">
+        <v>109</v>
+      </c>
+      <c r="AE40">
         <v>27.77920816140629</v>
       </c>
-      <c r="Y40">
-        <v>10.68431083131011</v>
-      </c>
-      <c r="Z40">
+      <c r="AF40">
+        <v>9.808197343142682</v>
+      </c>
+      <c r="AG40">
         <v>2.703657732989137</v>
       </c>
-      <c r="AA40">
-        <v>0.1070567945297273</v>
-      </c>
-      <c r="AB40">
-        <v>138.902908080254</v>
+      <c r="AH40">
+        <v>0.09827813737828967</v>
+      </c>
+      <c r="AI40">
+        <v>138.8985187516783</v>
       </c>
     </row>
-    <row r="41" spans="1:28">
+    <row r="41" spans="1:35">
       <c r="A41" s="1">
         <v>81</v>
       </c>
@@ -4126,10 +4168,10 @@
         <v>83</v>
       </c>
       <c r="C41" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D41" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="E41">
         <v>98.8</v>
@@ -4174,37 +4216,37 @@
         <v>145.17960793</v>
       </c>
       <c r="S41">
-        <v>0.2039425675844224</v>
+        <v>0.2039254030615986</v>
       </c>
       <c r="T41" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U41" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V41" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="W41" t="s">
-        <v>102</v>
-      </c>
-      <c r="X41">
+        <v>109</v>
+      </c>
+      <c r="AE41">
         <v>28.00341393636858</v>
       </c>
-      <c r="Y41">
-        <v>10.77054382168022</v>
-      </c>
-      <c r="Z41">
+      <c r="AF41">
+        <v>9.887359228302445</v>
+      </c>
+      <c r="AG41">
         <v>2.767110675765701</v>
       </c>
-      <c r="AA41">
-        <v>0.1073823219021518</v>
-      </c>
-      <c r="AB41">
-        <v>148.0004097667168</v>
+      <c r="AH41">
+        <v>0.09857697150617539</v>
+      </c>
+      <c r="AI41">
+        <v>147.9960070915188</v>
       </c>
     </row>
-    <row r="42" spans="1:28">
+    <row r="42" spans="1:35">
       <c r="A42" s="1">
         <v>83</v>
       </c>
@@ -4212,10 +4254,10 @@
         <v>85</v>
       </c>
       <c r="C42" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D42" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="E42">
         <v>93.92666666666666</v>
@@ -4236,7 +4278,7 @@
         <v>43785</v>
       </c>
       <c r="K42">
-        <v>-22.5</v>
+        <v>-23.5</v>
       </c>
       <c r="L42">
         <v>9.960000000000001</v>
@@ -4260,37 +4302,37 @@
         <v>714.756704585</v>
       </c>
       <c r="S42">
-        <v>2.448487140907533</v>
+        <v>2.448469944865225</v>
       </c>
       <c r="T42" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U42" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="V42" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="W42" t="s">
-        <v>102</v>
-      </c>
-      <c r="X42">
+        <v>109</v>
+      </c>
+      <c r="AE42">
         <v>27.85882252757645</v>
       </c>
-      <c r="Y42">
-        <v>10.71493174137555</v>
-      </c>
-      <c r="Z42">
+      <c r="AF42">
+        <v>9.83630733858276</v>
+      </c>
+      <c r="AG42">
         <v>2.616686337273497</v>
       </c>
-      <c r="AA42">
-        <v>0.1067207201441005</v>
-      </c>
-      <c r="AB42">
-        <v>717.4267512823455</v>
+      <c r="AH42">
+        <v>0.09796962109228431</v>
+      </c>
+      <c r="AI42">
+        <v>717.4223757328197</v>
       </c>
     </row>
-    <row r="43" spans="1:28">
+    <row r="43" spans="1:35">
       <c r="A43" s="1">
         <v>84</v>
       </c>
@@ -4298,10 +4340,10 @@
         <v>86</v>
       </c>
       <c r="C43" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D43" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E43">
         <v>89.39999999999999</v>
@@ -4322,7 +4364,7 @@
         <v>43785</v>
       </c>
       <c r="K43">
-        <v>-22.5</v>
+        <v>-23.5</v>
       </c>
       <c r="L43">
         <v>10.03</v>
@@ -4346,37 +4388,37 @@
         <v>804.62974851</v>
       </c>
       <c r="S43">
-        <v>2.788400020465609</v>
+        <v>2.788382760835358</v>
       </c>
       <c r="T43" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U43" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V43" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="W43" t="s">
-        <v>102</v>
-      </c>
-      <c r="X43">
+        <v>109</v>
+      </c>
+      <c r="AE43">
         <v>27.94603118461817</v>
       </c>
-      <c r="Y43">
-        <v>10.74847353254545</v>
-      </c>
-      <c r="Z43">
+      <c r="AF43">
+        <v>9.867098702876723</v>
+      </c>
+      <c r="AG43">
         <v>2.560042763385588</v>
       </c>
-      <c r="AA43">
-        <v>0.1078071895314308</v>
-      </c>
-      <c r="AB43">
-        <v>807.2436948681514</v>
+      <c r="AH43">
+        <v>0.09896699998985352</v>
+      </c>
+      <c r="AI43">
+        <v>807.2392747733805</v>
       </c>
     </row>
-    <row r="44" spans="1:28">
+    <row r="44" spans="1:35">
       <c r="A44" s="1">
         <v>88</v>
       </c>
@@ -4384,10 +4426,10 @@
         <v>90</v>
       </c>
       <c r="C44" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D44" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E44">
         <v>102.02</v>
@@ -4408,7 +4450,7 @@
         <v>43785</v>
       </c>
       <c r="K44">
-        <v>-22.5</v>
+        <v>-23.5</v>
       </c>
       <c r="L44">
         <v>9.98</v>
@@ -4432,37 +4474,37 @@
         <v>725.3135633099999</v>
       </c>
       <c r="S44">
-        <v>2.458629495579792</v>
+        <v>2.458612326550329</v>
       </c>
       <c r="T44" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U44" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="V44" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="W44" t="s">
-        <v>102</v>
-      </c>
-      <c r="X44">
+        <v>109</v>
+      </c>
+      <c r="AE44">
         <v>28.03087866541393</v>
       </c>
-      <c r="Y44">
-        <v>10.78110717900536</v>
-      </c>
-      <c r="Z44">
+      <c r="AF44">
+        <v>9.897056390326918</v>
+      </c>
+      <c r="AG44">
         <v>2.859710241445529</v>
       </c>
-      <c r="AA44">
-        <v>0.1075954496464735</v>
-      </c>
-      <c r="AB44">
-        <v>728.2270712762687</v>
+      <c r="AH44">
+        <v>0.09877262277546266</v>
+      </c>
+      <c r="AI44">
+        <v>728.2226598628332</v>
       </c>
     </row>
-    <row r="45" spans="1:28">
+    <row r="45" spans="1:35">
       <c r="A45" s="1">
         <v>89</v>
       </c>
@@ -4470,10 +4512,10 @@
         <v>91</v>
       </c>
       <c r="C45" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D45" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="E45">
         <v>90.51666666666667</v>
@@ -4494,7 +4536,7 @@
         <v>43785</v>
       </c>
       <c r="K45">
-        <v>-22.5</v>
+        <v>-23.5</v>
       </c>
       <c r="L45">
         <v>10.02</v>
@@ -4518,37 +4560,37 @@
         <v>760.5733733850001</v>
       </c>
       <c r="S45">
-        <v>2.616892808427253</v>
+        <v>2.616875563229956</v>
       </c>
       <c r="T45" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U45" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="V45" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="W45" t="s">
-        <v>102</v>
-      </c>
-      <c r="X45">
+        <v>109</v>
+      </c>
+      <c r="AE45">
         <v>27.95101865280697</v>
       </c>
-      <c r="Y45">
-        <v>10.75039178954114</v>
-      </c>
-      <c r="Z45">
+      <c r="AF45">
+        <v>9.868859662798767</v>
+      </c>
+      <c r="AG45">
         <v>2.530033038389911</v>
       </c>
-      <c r="AA45">
-        <v>0.1077189257312022</v>
-      </c>
-      <c r="AB45">
-        <v>763.1572658862556</v>
+      <c r="AH45">
+        <v>0.09888597382124364</v>
+      </c>
+      <c r="AI45">
+        <v>763.1528494103006</v>
       </c>
     </row>
-    <row r="46" spans="1:28">
+    <row r="46" spans="1:35">
       <c r="A46" s="1">
         <v>93</v>
       </c>
@@ -4556,10 +4598,10 @@
         <v>95</v>
       </c>
       <c r="C46" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="D46" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="E46">
         <v>94.28000000000002</v>
@@ -4580,7 +4622,7 @@
         <v>43787</v>
       </c>
       <c r="K46">
-        <v>-24.6</v>
+        <v>-23.5</v>
       </c>
       <c r="L46">
         <v>10.18</v>
@@ -4604,37 +4646,37 @@
         <v>800.133399485</v>
       </c>
       <c r="S46">
-        <v>2.765744421781582</v>
+        <v>2.765726965099131</v>
       </c>
       <c r="T46" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U46" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V46" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="W46" t="s">
-        <v>102</v>
-      </c>
-      <c r="X46">
+        <v>109</v>
+      </c>
+      <c r="AE46">
         <v>27.93107145012167</v>
       </c>
-      <c r="Y46">
-        <v>10.74271978850834</v>
-      </c>
-      <c r="Z46">
+      <c r="AF46">
+        <v>9.861816765850653</v>
+      </c>
+      <c r="AG46">
         <v>2.643675912754016</v>
       </c>
-      <c r="AA46">
-        <v>0.1093608874470148</v>
-      </c>
-      <c r="AB46">
-        <v>802.8317558414776</v>
+      <c r="AH46">
+        <v>0.1003932946763596</v>
+      </c>
+      <c r="AI46">
+        <v>802.8272720450923</v>
       </c>
     </row>
-    <row r="47" spans="1:28">
+    <row r="47" spans="1:35">
       <c r="A47" s="1">
         <v>95</v>
       </c>
@@ -4642,10 +4684,10 @@
         <v>97</v>
       </c>
       <c r="C47" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D47" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="E47">
         <v>98.8</v>
@@ -4666,7 +4708,7 @@
         <v>43787</v>
       </c>
       <c r="K47">
-        <v>-25</v>
+        <v>-23.5</v>
       </c>
       <c r="L47">
         <v>10.16</v>
@@ -4690,37 +4732,37 @@
         <v>834.546895665</v>
       </c>
       <c r="S47">
-        <v>2.885131709023637</v>
+        <v>2.885114300416533</v>
       </c>
       <c r="T47" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U47" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V47" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="W47" t="s">
-        <v>102</v>
-      </c>
-      <c r="X47">
+        <v>109</v>
+      </c>
+      <c r="AE47">
         <v>28.00341393636858</v>
       </c>
-      <c r="Y47">
-        <v>10.77054382168022</v>
-      </c>
-      <c r="Z47">
+      <c r="AF47">
+        <v>9.887359228302445</v>
+      </c>
+      <c r="AG47">
         <v>2.767110675765701</v>
       </c>
-      <c r="AA47">
-        <v>0.1094287252282711</v>
-      </c>
-      <c r="AB47">
-        <v>837.3687207033798</v>
+      <c r="AH47">
+        <v>0.1004555697595528</v>
+      </c>
+      <c r="AI47">
+        <v>837.3642341256455</v>
       </c>
     </row>
-    <row r="48" spans="1:28">
+    <row r="48" spans="1:35">
       <c r="A48" s="1">
         <v>96</v>
       </c>
@@ -4728,10 +4770,10 @@
         <v>98</v>
       </c>
       <c r="C48" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D48" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="E48">
         <v>96.52</v>
@@ -4752,7 +4794,7 @@
         <v>43787</v>
       </c>
       <c r="K48">
-        <v>-25</v>
+        <v>-23.5</v>
       </c>
       <c r="L48">
         <v>10.38</v>
@@ -4776,34 +4818,34 @@
         <v>710.7801080099999</v>
       </c>
       <c r="S48">
-        <v>2.431012891184941</v>
+        <v>2.430995132599475</v>
       </c>
       <c r="T48" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="U48" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V48" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="W48" t="s">
-        <v>102</v>
-      </c>
-      <c r="X48">
+        <v>109</v>
+      </c>
+      <c r="AE48">
         <v>27.77920816140629</v>
       </c>
-      <c r="Y48">
-        <v>10.68431083131011</v>
-      </c>
-      <c r="Z48">
+      <c r="AF48">
+        <v>9.808197343142682</v>
+      </c>
+      <c r="AG48">
         <v>2.703657732989137</v>
       </c>
-      <c r="AA48">
-        <v>0.110903146428999</v>
-      </c>
-      <c r="AB48">
-        <v>713.5392173162036</v>
+      <c r="AH48">
+        <v>0.101809088421821</v>
+      </c>
+      <c r="AI48">
+        <v>713.5346702872</v>
       </c>
     </row>
   </sheetData>

</xml_diff>